<commit_message>
feat(estandarizar_geo_cod): added complete DIVIPOLA standart into mpios
</commit_message>
<xml_diff>
--- a/inst/extdata/divipola_data.xlsx
+++ b/inst/extdata/divipola_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geral\Documents\TRACE\fixing\sivirep\inst\extdata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A661E44-742E-41E2-B070-5F5220A213EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3240A194-7D06-47CD-BCD9-81F895F69B27}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{AC01F1B4-24A3-41A4-89CD-B92F273F17AF}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3516" uniqueCount="1069">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3664" uniqueCount="1217">
   <si>
     <t>nombre_departamento</t>
   </si>
@@ -3243,6 +3243,450 @@
   </si>
   <si>
     <t>bogota</t>
+  </si>
+  <si>
+    <t>05001</t>
+  </si>
+  <si>
+    <t>05002</t>
+  </si>
+  <si>
+    <t>05004</t>
+  </si>
+  <si>
+    <t>05021</t>
+  </si>
+  <si>
+    <t>05030</t>
+  </si>
+  <si>
+    <t>05031</t>
+  </si>
+  <si>
+    <t>05034</t>
+  </si>
+  <si>
+    <t>05036</t>
+  </si>
+  <si>
+    <t>05038</t>
+  </si>
+  <si>
+    <t>05040</t>
+  </si>
+  <si>
+    <t>05042</t>
+  </si>
+  <si>
+    <t>05044</t>
+  </si>
+  <si>
+    <t>05045</t>
+  </si>
+  <si>
+    <t>05051</t>
+  </si>
+  <si>
+    <t>05055</t>
+  </si>
+  <si>
+    <t>05059</t>
+  </si>
+  <si>
+    <t>05079</t>
+  </si>
+  <si>
+    <t>05086</t>
+  </si>
+  <si>
+    <t>05088</t>
+  </si>
+  <si>
+    <t>05091</t>
+  </si>
+  <si>
+    <t>05093</t>
+  </si>
+  <si>
+    <t>05101</t>
+  </si>
+  <si>
+    <t>05107</t>
+  </si>
+  <si>
+    <t>05113</t>
+  </si>
+  <si>
+    <t>05120</t>
+  </si>
+  <si>
+    <t>05125</t>
+  </si>
+  <si>
+    <t>05129</t>
+  </si>
+  <si>
+    <t>05134</t>
+  </si>
+  <si>
+    <t>05138</t>
+  </si>
+  <si>
+    <t>05142</t>
+  </si>
+  <si>
+    <t>05145</t>
+  </si>
+  <si>
+    <t>05147</t>
+  </si>
+  <si>
+    <t>05148</t>
+  </si>
+  <si>
+    <t>05150</t>
+  </si>
+  <si>
+    <t>05154</t>
+  </si>
+  <si>
+    <t>05172</t>
+  </si>
+  <si>
+    <t>05190</t>
+  </si>
+  <si>
+    <t>05197</t>
+  </si>
+  <si>
+    <t>05206</t>
+  </si>
+  <si>
+    <t>05209</t>
+  </si>
+  <si>
+    <t>05212</t>
+  </si>
+  <si>
+    <t>05234</t>
+  </si>
+  <si>
+    <t>05237</t>
+  </si>
+  <si>
+    <t>05240</t>
+  </si>
+  <si>
+    <t>05250</t>
+  </si>
+  <si>
+    <t>05264</t>
+  </si>
+  <si>
+    <t>05266</t>
+  </si>
+  <si>
+    <t>05282</t>
+  </si>
+  <si>
+    <t>05284</t>
+  </si>
+  <si>
+    <t>05306</t>
+  </si>
+  <si>
+    <t>05308</t>
+  </si>
+  <si>
+    <t>05310</t>
+  </si>
+  <si>
+    <t>05313</t>
+  </si>
+  <si>
+    <t>05315</t>
+  </si>
+  <si>
+    <t>05318</t>
+  </si>
+  <si>
+    <t>05321</t>
+  </si>
+  <si>
+    <t>05347</t>
+  </si>
+  <si>
+    <t>05353</t>
+  </si>
+  <si>
+    <t>05360</t>
+  </si>
+  <si>
+    <t>05361</t>
+  </si>
+  <si>
+    <t>05364</t>
+  </si>
+  <si>
+    <t>05368</t>
+  </si>
+  <si>
+    <t>05376</t>
+  </si>
+  <si>
+    <t>05380</t>
+  </si>
+  <si>
+    <t>05390</t>
+  </si>
+  <si>
+    <t>05400</t>
+  </si>
+  <si>
+    <t>05411</t>
+  </si>
+  <si>
+    <t>05425</t>
+  </si>
+  <si>
+    <t>05440</t>
+  </si>
+  <si>
+    <t>05467</t>
+  </si>
+  <si>
+    <t>05475</t>
+  </si>
+  <si>
+    <t>05480</t>
+  </si>
+  <si>
+    <t>05483</t>
+  </si>
+  <si>
+    <t>05490</t>
+  </si>
+  <si>
+    <t>05495</t>
+  </si>
+  <si>
+    <t>05501</t>
+  </si>
+  <si>
+    <t>05541</t>
+  </si>
+  <si>
+    <t>05543</t>
+  </si>
+  <si>
+    <t>05576</t>
+  </si>
+  <si>
+    <t>05579</t>
+  </si>
+  <si>
+    <t>05585</t>
+  </si>
+  <si>
+    <t>05591</t>
+  </si>
+  <si>
+    <t>05604</t>
+  </si>
+  <si>
+    <t>05607</t>
+  </si>
+  <si>
+    <t>05615</t>
+  </si>
+  <si>
+    <t>05628</t>
+  </si>
+  <si>
+    <t>05631</t>
+  </si>
+  <si>
+    <t>05642</t>
+  </si>
+  <si>
+    <t>05647</t>
+  </si>
+  <si>
+    <t>05649</t>
+  </si>
+  <si>
+    <t>05652</t>
+  </si>
+  <si>
+    <t>05656</t>
+  </si>
+  <si>
+    <t>05658</t>
+  </si>
+  <si>
+    <t>05659</t>
+  </si>
+  <si>
+    <t>05660</t>
+  </si>
+  <si>
+    <t>05664</t>
+  </si>
+  <si>
+    <t>05665</t>
+  </si>
+  <si>
+    <t>05667</t>
+  </si>
+  <si>
+    <t>05670</t>
+  </si>
+  <si>
+    <t>05674</t>
+  </si>
+  <si>
+    <t>05679</t>
+  </si>
+  <si>
+    <t>05686</t>
+  </si>
+  <si>
+    <t>05690</t>
+  </si>
+  <si>
+    <t>05697</t>
+  </si>
+  <si>
+    <t>05736</t>
+  </si>
+  <si>
+    <t>05756</t>
+  </si>
+  <si>
+    <t>05761</t>
+  </si>
+  <si>
+    <t>05789</t>
+  </si>
+  <si>
+    <t>05790</t>
+  </si>
+  <si>
+    <t>05792</t>
+  </si>
+  <si>
+    <t>05809</t>
+  </si>
+  <si>
+    <t>05819</t>
+  </si>
+  <si>
+    <t>05837</t>
+  </si>
+  <si>
+    <t>05842</t>
+  </si>
+  <si>
+    <t>05847</t>
+  </si>
+  <si>
+    <t>05854</t>
+  </si>
+  <si>
+    <t>05856</t>
+  </si>
+  <si>
+    <t>05858</t>
+  </si>
+  <si>
+    <t>05861</t>
+  </si>
+  <si>
+    <t>05873</t>
+  </si>
+  <si>
+    <t>05885</t>
+  </si>
+  <si>
+    <t>05887</t>
+  </si>
+  <si>
+    <t>05890</t>
+  </si>
+  <si>
+    <t>05893</t>
+  </si>
+  <si>
+    <t>05895</t>
+  </si>
+  <si>
+    <t>08001</t>
+  </si>
+  <si>
+    <t>08078</t>
+  </si>
+  <si>
+    <t>08137</t>
+  </si>
+  <si>
+    <t>08141</t>
+  </si>
+  <si>
+    <t>08296</t>
+  </si>
+  <si>
+    <t>08372</t>
+  </si>
+  <si>
+    <t>08421</t>
+  </si>
+  <si>
+    <t>08433</t>
+  </si>
+  <si>
+    <t>08436</t>
+  </si>
+  <si>
+    <t>08520</t>
+  </si>
+  <si>
+    <t>08549</t>
+  </si>
+  <si>
+    <t>08558</t>
+  </si>
+  <si>
+    <t>08560</t>
+  </si>
+  <si>
+    <t>08573</t>
+  </si>
+  <si>
+    <t>08606</t>
+  </si>
+  <si>
+    <t>08634</t>
+  </si>
+  <si>
+    <t>08638</t>
+  </si>
+  <si>
+    <t>08675</t>
+  </si>
+  <si>
+    <t>08685</t>
+  </si>
+  <si>
+    <t>08758</t>
+  </si>
+  <si>
+    <t>08770</t>
+  </si>
+  <si>
+    <t>08832</t>
+  </si>
+  <si>
+    <t>08849</t>
   </si>
 </sst>
 </file>
@@ -3299,7 +3743,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -3315,6 +3759,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -3632,11 +4079,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9DD52B2-7198-4BE0-B28C-138C9105CC1D}">
   <dimension ref="A1:E1122"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1103" workbookViewId="0">
-      <selection activeCell="E1124" sqref="E1124"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="9.109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
@@ -3659,8 +4109,8 @@
       <c r="A2" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B2" s="4">
-        <v>5001</v>
+      <c r="B2" s="6" t="s">
+        <v>1069</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>5</v>
@@ -3676,8 +4126,8 @@
       <c r="A3" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B3" s="4">
-        <v>5002</v>
+      <c r="B3" s="6" t="s">
+        <v>1070</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>5</v>
@@ -3693,8 +4143,8 @@
       <c r="A4" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B4" s="4">
-        <v>5004</v>
+      <c r="B4" s="6" t="s">
+        <v>1071</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>5</v>
@@ -3710,8 +4160,8 @@
       <c r="A5" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B5" s="4">
-        <v>5021</v>
+      <c r="B5" s="6" t="s">
+        <v>1072</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>5</v>
@@ -3727,8 +4177,8 @@
       <c r="A6" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B6" s="4">
-        <v>5030</v>
+      <c r="B6" s="6" t="s">
+        <v>1073</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>5</v>
@@ -3744,8 +4194,8 @@
       <c r="A7" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B7" s="4">
-        <v>5031</v>
+      <c r="B7" s="6" t="s">
+        <v>1074</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>5</v>
@@ -3761,8 +4211,8 @@
       <c r="A8" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B8" s="4">
-        <v>5034</v>
+      <c r="B8" s="6" t="s">
+        <v>1075</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>5</v>
@@ -3778,8 +4228,8 @@
       <c r="A9" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B9" s="4">
-        <v>5036</v>
+      <c r="B9" s="6" t="s">
+        <v>1076</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>5</v>
@@ -3795,8 +4245,8 @@
       <c r="A10" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B10" s="4">
-        <v>5038</v>
+      <c r="B10" s="6" t="s">
+        <v>1077</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>5</v>
@@ -3812,8 +4262,8 @@
       <c r="A11" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B11" s="4">
-        <v>5040</v>
+      <c r="B11" s="6" t="s">
+        <v>1078</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>5</v>
@@ -3829,8 +4279,8 @@
       <c r="A12" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B12" s="4">
-        <v>5042</v>
+      <c r="B12" s="6" t="s">
+        <v>1079</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>5</v>
@@ -3846,8 +4296,8 @@
       <c r="A13" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B13" s="4">
-        <v>5044</v>
+      <c r="B13" s="6" t="s">
+        <v>1080</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>5</v>
@@ -3863,8 +4313,8 @@
       <c r="A14" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B14" s="4">
-        <v>5045</v>
+      <c r="B14" s="6" t="s">
+        <v>1081</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>5</v>
@@ -3880,8 +4330,8 @@
       <c r="A15" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B15" s="4">
-        <v>5051</v>
+      <c r="B15" s="6" t="s">
+        <v>1082</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>5</v>
@@ -3897,8 +4347,8 @@
       <c r="A16" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B16" s="4">
-        <v>5055</v>
+      <c r="B16" s="6" t="s">
+        <v>1083</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>5</v>
@@ -3914,8 +4364,8 @@
       <c r="A17" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B17" s="4">
-        <v>5059</v>
+      <c r="B17" s="6" t="s">
+        <v>1084</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>5</v>
@@ -3931,8 +4381,8 @@
       <c r="A18" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B18" s="4">
-        <v>5079</v>
+      <c r="B18" s="6" t="s">
+        <v>1085</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>5</v>
@@ -3948,8 +4398,8 @@
       <c r="A19" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B19" s="4">
-        <v>5086</v>
+      <c r="B19" s="6" t="s">
+        <v>1086</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>5</v>
@@ -3965,8 +4415,8 @@
       <c r="A20" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B20" s="4">
-        <v>5088</v>
+      <c r="B20" s="6" t="s">
+        <v>1087</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>5</v>
@@ -3982,8 +4432,8 @@
       <c r="A21" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B21" s="4">
-        <v>5091</v>
+      <c r="B21" s="6" t="s">
+        <v>1088</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>5</v>
@@ -3999,8 +4449,8 @@
       <c r="A22" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B22" s="4">
-        <v>5093</v>
+      <c r="B22" s="6" t="s">
+        <v>1089</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>5</v>
@@ -4016,8 +4466,8 @@
       <c r="A23" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B23" s="4">
-        <v>5101</v>
+      <c r="B23" s="6" t="s">
+        <v>1090</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>5</v>
@@ -4033,8 +4483,8 @@
       <c r="A24" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B24" s="4">
-        <v>5107</v>
+      <c r="B24" s="6" t="s">
+        <v>1091</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>5</v>
@@ -4050,8 +4500,8 @@
       <c r="A25" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B25" s="4">
-        <v>5113</v>
+      <c r="B25" s="6" t="s">
+        <v>1092</v>
       </c>
       <c r="C25" s="3" t="s">
         <v>5</v>
@@ -4067,8 +4517,8 @@
       <c r="A26" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B26" s="4">
-        <v>5120</v>
+      <c r="B26" s="6" t="s">
+        <v>1093</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>5</v>
@@ -4084,8 +4534,8 @@
       <c r="A27" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B27" s="4">
-        <v>5125</v>
+      <c r="B27" s="6" t="s">
+        <v>1094</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>5</v>
@@ -4101,8 +4551,8 @@
       <c r="A28" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B28" s="4">
-        <v>5129</v>
+      <c r="B28" s="6" t="s">
+        <v>1095</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>5</v>
@@ -4118,8 +4568,8 @@
       <c r="A29" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B29" s="4">
-        <v>5134</v>
+      <c r="B29" s="6" t="s">
+        <v>1096</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>5</v>
@@ -4135,8 +4585,8 @@
       <c r="A30" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B30" s="4">
-        <v>5138</v>
+      <c r="B30" s="6" t="s">
+        <v>1097</v>
       </c>
       <c r="C30" s="3" t="s">
         <v>5</v>
@@ -4152,8 +4602,8 @@
       <c r="A31" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B31" s="4">
-        <v>5142</v>
+      <c r="B31" s="6" t="s">
+        <v>1098</v>
       </c>
       <c r="C31" s="3" t="s">
         <v>5</v>
@@ -4169,8 +4619,8 @@
       <c r="A32" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B32" s="4">
-        <v>5145</v>
+      <c r="B32" s="6" t="s">
+        <v>1099</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>5</v>
@@ -4186,8 +4636,8 @@
       <c r="A33" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B33" s="4">
-        <v>5147</v>
+      <c r="B33" s="6" t="s">
+        <v>1100</v>
       </c>
       <c r="C33" s="3" t="s">
         <v>5</v>
@@ -4203,8 +4653,8 @@
       <c r="A34" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B34" s="4">
-        <v>5148</v>
+      <c r="B34" s="6" t="s">
+        <v>1101</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>5</v>
@@ -4220,8 +4670,8 @@
       <c r="A35" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B35" s="4">
-        <v>5150</v>
+      <c r="B35" s="6" t="s">
+        <v>1102</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>5</v>
@@ -4237,8 +4687,8 @@
       <c r="A36" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B36" s="4">
-        <v>5154</v>
+      <c r="B36" s="6" t="s">
+        <v>1103</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>5</v>
@@ -4254,8 +4704,8 @@
       <c r="A37" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B37" s="4">
-        <v>5172</v>
+      <c r="B37" s="6" t="s">
+        <v>1104</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>5</v>
@@ -4271,8 +4721,8 @@
       <c r="A38" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B38" s="4">
-        <v>5190</v>
+      <c r="B38" s="6" t="s">
+        <v>1105</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>5</v>
@@ -4288,8 +4738,8 @@
       <c r="A39" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B39" s="4">
-        <v>5197</v>
+      <c r="B39" s="6" t="s">
+        <v>1106</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>5</v>
@@ -4305,8 +4755,8 @@
       <c r="A40" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B40" s="4">
-        <v>5206</v>
+      <c r="B40" s="6" t="s">
+        <v>1107</v>
       </c>
       <c r="C40" s="3" t="s">
         <v>5</v>
@@ -4322,8 +4772,8 @@
       <c r="A41" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B41" s="4">
-        <v>5209</v>
+      <c r="B41" s="6" t="s">
+        <v>1108</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>5</v>
@@ -4339,8 +4789,8 @@
       <c r="A42" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B42" s="4">
-        <v>5212</v>
+      <c r="B42" s="6" t="s">
+        <v>1109</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>5</v>
@@ -4356,8 +4806,8 @@
       <c r="A43" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B43" s="4">
-        <v>5234</v>
+      <c r="B43" s="6" t="s">
+        <v>1110</v>
       </c>
       <c r="C43" s="3" t="s">
         <v>5</v>
@@ -4373,8 +4823,8 @@
       <c r="A44" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B44" s="4">
-        <v>5237</v>
+      <c r="B44" s="6" t="s">
+        <v>1111</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>5</v>
@@ -4390,8 +4840,8 @@
       <c r="A45" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B45" s="4">
-        <v>5240</v>
+      <c r="B45" s="6" t="s">
+        <v>1112</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>5</v>
@@ -4407,8 +4857,8 @@
       <c r="A46" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B46" s="4">
-        <v>5250</v>
+      <c r="B46" s="6" t="s">
+        <v>1113</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>5</v>
@@ -4424,8 +4874,8 @@
       <c r="A47" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B47" s="4">
-        <v>5264</v>
+      <c r="B47" s="6" t="s">
+        <v>1114</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>5</v>
@@ -4441,8 +4891,8 @@
       <c r="A48" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B48" s="4">
-        <v>5266</v>
+      <c r="B48" s="6" t="s">
+        <v>1115</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>5</v>
@@ -4458,8 +4908,8 @@
       <c r="A49" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B49" s="4">
-        <v>5282</v>
+      <c r="B49" s="6" t="s">
+        <v>1116</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>5</v>
@@ -4475,8 +4925,8 @@
       <c r="A50" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B50" s="4">
-        <v>5284</v>
+      <c r="B50" s="6" t="s">
+        <v>1117</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>5</v>
@@ -4492,8 +4942,8 @@
       <c r="A51" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B51" s="4">
-        <v>5306</v>
+      <c r="B51" s="6" t="s">
+        <v>1118</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>5</v>
@@ -4509,8 +4959,8 @@
       <c r="A52" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B52" s="4">
-        <v>5308</v>
+      <c r="B52" s="6" t="s">
+        <v>1119</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>5</v>
@@ -4526,8 +4976,8 @@
       <c r="A53" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B53" s="4">
-        <v>5310</v>
+      <c r="B53" s="6" t="s">
+        <v>1120</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>5</v>
@@ -4543,8 +4993,8 @@
       <c r="A54" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B54" s="4">
-        <v>5313</v>
+      <c r="B54" s="6" t="s">
+        <v>1121</v>
       </c>
       <c r="C54" s="3" t="s">
         <v>5</v>
@@ -4560,8 +5010,8 @@
       <c r="A55" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B55" s="4">
-        <v>5315</v>
+      <c r="B55" s="6" t="s">
+        <v>1122</v>
       </c>
       <c r="C55" s="3" t="s">
         <v>5</v>
@@ -4577,8 +5027,8 @@
       <c r="A56" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B56" s="4">
-        <v>5318</v>
+      <c r="B56" s="6" t="s">
+        <v>1123</v>
       </c>
       <c r="C56" s="3" t="s">
         <v>5</v>
@@ -4594,8 +5044,8 @@
       <c r="A57" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B57" s="4">
-        <v>5321</v>
+      <c r="B57" s="6" t="s">
+        <v>1124</v>
       </c>
       <c r="C57" s="3" t="s">
         <v>5</v>
@@ -4611,8 +5061,8 @@
       <c r="A58" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B58" s="4">
-        <v>5347</v>
+      <c r="B58" s="6" t="s">
+        <v>1125</v>
       </c>
       <c r="C58" s="3" t="s">
         <v>5</v>
@@ -4628,8 +5078,8 @@
       <c r="A59" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B59" s="4">
-        <v>5353</v>
+      <c r="B59" s="6" t="s">
+        <v>1126</v>
       </c>
       <c r="C59" s="3" t="s">
         <v>5</v>
@@ -4645,8 +5095,8 @@
       <c r="A60" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B60" s="4">
-        <v>5360</v>
+      <c r="B60" s="6" t="s">
+        <v>1127</v>
       </c>
       <c r="C60" s="3" t="s">
         <v>5</v>
@@ -4662,8 +5112,8 @@
       <c r="A61" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B61" s="4">
-        <v>5361</v>
+      <c r="B61" s="6" t="s">
+        <v>1128</v>
       </c>
       <c r="C61" s="3" t="s">
         <v>5</v>
@@ -4679,8 +5129,8 @@
       <c r="A62" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B62" s="4">
-        <v>5364</v>
+      <c r="B62" s="6" t="s">
+        <v>1129</v>
       </c>
       <c r="C62" s="3" t="s">
         <v>5</v>
@@ -4696,8 +5146,8 @@
       <c r="A63" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B63" s="4">
-        <v>5368</v>
+      <c r="B63" s="6" t="s">
+        <v>1130</v>
       </c>
       <c r="C63" s="3" t="s">
         <v>5</v>
@@ -4713,8 +5163,8 @@
       <c r="A64" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B64" s="4">
-        <v>5376</v>
+      <c r="B64" s="6" t="s">
+        <v>1131</v>
       </c>
       <c r="C64" s="3" t="s">
         <v>5</v>
@@ -4730,8 +5180,8 @@
       <c r="A65" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B65" s="4">
-        <v>5380</v>
+      <c r="B65" s="6" t="s">
+        <v>1132</v>
       </c>
       <c r="C65" s="3" t="s">
         <v>5</v>
@@ -4747,8 +5197,8 @@
       <c r="A66" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B66" s="4">
-        <v>5390</v>
+      <c r="B66" s="6" t="s">
+        <v>1133</v>
       </c>
       <c r="C66" s="3" t="s">
         <v>5</v>
@@ -4764,8 +5214,8 @@
       <c r="A67" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B67" s="4">
-        <v>5400</v>
+      <c r="B67" s="6" t="s">
+        <v>1134</v>
       </c>
       <c r="C67" s="3" t="s">
         <v>5</v>
@@ -4781,8 +5231,8 @@
       <c r="A68" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B68" s="4">
-        <v>5411</v>
+      <c r="B68" s="6" t="s">
+        <v>1135</v>
       </c>
       <c r="C68" s="3" t="s">
         <v>5</v>
@@ -4798,8 +5248,8 @@
       <c r="A69" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B69" s="4">
-        <v>5425</v>
+      <c r="B69" s="6" t="s">
+        <v>1136</v>
       </c>
       <c r="C69" s="3" t="s">
         <v>5</v>
@@ -4815,8 +5265,8 @@
       <c r="A70" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B70" s="4">
-        <v>5440</v>
+      <c r="B70" s="6" t="s">
+        <v>1137</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>5</v>
@@ -4832,8 +5282,8 @@
       <c r="A71" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B71" s="4">
-        <v>5467</v>
+      <c r="B71" s="6" t="s">
+        <v>1138</v>
       </c>
       <c r="C71" s="3" t="s">
         <v>5</v>
@@ -4849,8 +5299,8 @@
       <c r="A72" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B72" s="4">
-        <v>5475</v>
+      <c r="B72" s="6" t="s">
+        <v>1139</v>
       </c>
       <c r="C72" s="3" t="s">
         <v>5</v>
@@ -4866,8 +5316,8 @@
       <c r="A73" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B73" s="4">
-        <v>5480</v>
+      <c r="B73" s="6" t="s">
+        <v>1140</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>5</v>
@@ -4883,8 +5333,8 @@
       <c r="A74" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B74" s="4">
-        <v>5483</v>
+      <c r="B74" s="6" t="s">
+        <v>1141</v>
       </c>
       <c r="C74" s="3" t="s">
         <v>5</v>
@@ -4900,8 +5350,8 @@
       <c r="A75" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B75" s="4">
-        <v>5490</v>
+      <c r="B75" s="6" t="s">
+        <v>1142</v>
       </c>
       <c r="C75" s="3" t="s">
         <v>5</v>
@@ -4917,8 +5367,8 @@
       <c r="A76" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B76" s="4">
-        <v>5495</v>
+      <c r="B76" s="6" t="s">
+        <v>1143</v>
       </c>
       <c r="C76" s="3" t="s">
         <v>5</v>
@@ -4934,8 +5384,8 @@
       <c r="A77" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B77" s="4">
-        <v>5501</v>
+      <c r="B77" s="6" t="s">
+        <v>1144</v>
       </c>
       <c r="C77" s="3" t="s">
         <v>5</v>
@@ -4951,8 +5401,8 @@
       <c r="A78" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B78" s="4">
-        <v>5541</v>
+      <c r="B78" s="6" t="s">
+        <v>1145</v>
       </c>
       <c r="C78" s="3" t="s">
         <v>5</v>
@@ -4968,8 +5418,8 @@
       <c r="A79" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B79" s="4">
-        <v>5543</v>
+      <c r="B79" s="6" t="s">
+        <v>1146</v>
       </c>
       <c r="C79" s="3" t="s">
         <v>5</v>
@@ -4985,8 +5435,8 @@
       <c r="A80" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B80" s="4">
-        <v>5576</v>
+      <c r="B80" s="6" t="s">
+        <v>1147</v>
       </c>
       <c r="C80" s="3" t="s">
         <v>5</v>
@@ -5002,8 +5452,8 @@
       <c r="A81" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B81" s="4">
-        <v>5579</v>
+      <c r="B81" s="6" t="s">
+        <v>1148</v>
       </c>
       <c r="C81" s="3" t="s">
         <v>5</v>
@@ -5019,8 +5469,8 @@
       <c r="A82" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B82" s="4">
-        <v>5585</v>
+      <c r="B82" s="6" t="s">
+        <v>1149</v>
       </c>
       <c r="C82" s="3" t="s">
         <v>5</v>
@@ -5036,8 +5486,8 @@
       <c r="A83" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B83" s="4">
-        <v>5591</v>
+      <c r="B83" s="6" t="s">
+        <v>1150</v>
       </c>
       <c r="C83" s="3" t="s">
         <v>5</v>
@@ -5053,8 +5503,8 @@
       <c r="A84" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B84" s="4">
-        <v>5604</v>
+      <c r="B84" s="6" t="s">
+        <v>1151</v>
       </c>
       <c r="C84" s="3" t="s">
         <v>5</v>
@@ -5070,8 +5520,8 @@
       <c r="A85" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B85" s="4">
-        <v>5607</v>
+      <c r="B85" s="6" t="s">
+        <v>1152</v>
       </c>
       <c r="C85" s="3" t="s">
         <v>5</v>
@@ -5087,8 +5537,8 @@
       <c r="A86" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B86" s="4">
-        <v>5615</v>
+      <c r="B86" s="6" t="s">
+        <v>1153</v>
       </c>
       <c r="C86" s="3" t="s">
         <v>5</v>
@@ -5104,8 +5554,8 @@
       <c r="A87" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B87" s="4">
-        <v>5628</v>
+      <c r="B87" s="6" t="s">
+        <v>1154</v>
       </c>
       <c r="C87" s="3" t="s">
         <v>5</v>
@@ -5121,8 +5571,8 @@
       <c r="A88" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B88" s="4">
-        <v>5631</v>
+      <c r="B88" s="6" t="s">
+        <v>1155</v>
       </c>
       <c r="C88" s="3" t="s">
         <v>5</v>
@@ -5138,8 +5588,8 @@
       <c r="A89" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B89" s="4">
-        <v>5642</v>
+      <c r="B89" s="6" t="s">
+        <v>1156</v>
       </c>
       <c r="C89" s="3" t="s">
         <v>5</v>
@@ -5155,8 +5605,8 @@
       <c r="A90" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B90" s="4">
-        <v>5647</v>
+      <c r="B90" s="6" t="s">
+        <v>1157</v>
       </c>
       <c r="C90" s="3" t="s">
         <v>5</v>
@@ -5172,8 +5622,8 @@
       <c r="A91" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B91" s="4">
-        <v>5649</v>
+      <c r="B91" s="6" t="s">
+        <v>1158</v>
       </c>
       <c r="C91" s="3" t="s">
         <v>5</v>
@@ -5189,8 +5639,8 @@
       <c r="A92" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B92" s="4">
-        <v>5652</v>
+      <c r="B92" s="6" t="s">
+        <v>1159</v>
       </c>
       <c r="C92" s="3" t="s">
         <v>5</v>
@@ -5206,8 +5656,8 @@
       <c r="A93" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B93" s="4">
-        <v>5656</v>
+      <c r="B93" s="6" t="s">
+        <v>1160</v>
       </c>
       <c r="C93" s="3" t="s">
         <v>5</v>
@@ -5223,8 +5673,8 @@
       <c r="A94" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B94" s="4">
-        <v>5658</v>
+      <c r="B94" s="6" t="s">
+        <v>1161</v>
       </c>
       <c r="C94" s="3" t="s">
         <v>5</v>
@@ -5240,8 +5690,8 @@
       <c r="A95" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B95" s="4">
-        <v>5659</v>
+      <c r="B95" s="6" t="s">
+        <v>1162</v>
       </c>
       <c r="C95" s="3" t="s">
         <v>5</v>
@@ -5257,8 +5707,8 @@
       <c r="A96" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B96" s="4">
-        <v>5660</v>
+      <c r="B96" s="6" t="s">
+        <v>1163</v>
       </c>
       <c r="C96" s="3" t="s">
         <v>5</v>
@@ -5274,8 +5724,8 @@
       <c r="A97" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B97" s="4">
-        <v>5664</v>
+      <c r="B97" s="6" t="s">
+        <v>1164</v>
       </c>
       <c r="C97" s="3" t="s">
         <v>5</v>
@@ -5291,8 +5741,8 @@
       <c r="A98" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B98" s="4">
-        <v>5665</v>
+      <c r="B98" s="6" t="s">
+        <v>1165</v>
       </c>
       <c r="C98" s="3" t="s">
         <v>5</v>
@@ -5308,8 +5758,8 @@
       <c r="A99" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B99" s="4">
-        <v>5667</v>
+      <c r="B99" s="6" t="s">
+        <v>1166</v>
       </c>
       <c r="C99" s="3" t="s">
         <v>5</v>
@@ -5325,8 +5775,8 @@
       <c r="A100" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B100" s="4">
-        <v>5670</v>
+      <c r="B100" s="6" t="s">
+        <v>1167</v>
       </c>
       <c r="C100" s="3" t="s">
         <v>5</v>
@@ -5342,8 +5792,8 @@
       <c r="A101" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B101" s="4">
-        <v>5674</v>
+      <c r="B101" s="6" t="s">
+        <v>1168</v>
       </c>
       <c r="C101" s="3" t="s">
         <v>5</v>
@@ -5359,8 +5809,8 @@
       <c r="A102" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B102" s="4">
-        <v>5679</v>
+      <c r="B102" s="6" t="s">
+        <v>1169</v>
       </c>
       <c r="C102" s="3" t="s">
         <v>5</v>
@@ -5376,8 +5826,8 @@
       <c r="A103" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B103" s="4">
-        <v>5686</v>
+      <c r="B103" s="6" t="s">
+        <v>1170</v>
       </c>
       <c r="C103" s="3" t="s">
         <v>5</v>
@@ -5393,8 +5843,8 @@
       <c r="A104" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B104" s="4">
-        <v>5690</v>
+      <c r="B104" s="6" t="s">
+        <v>1171</v>
       </c>
       <c r="C104" s="3" t="s">
         <v>5</v>
@@ -5410,8 +5860,8 @@
       <c r="A105" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B105" s="4">
-        <v>5697</v>
+      <c r="B105" s="6" t="s">
+        <v>1172</v>
       </c>
       <c r="C105" s="3" t="s">
         <v>5</v>
@@ -5427,8 +5877,8 @@
       <c r="A106" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B106" s="4">
-        <v>5736</v>
+      <c r="B106" s="6" t="s">
+        <v>1173</v>
       </c>
       <c r="C106" s="3" t="s">
         <v>5</v>
@@ -5444,8 +5894,8 @@
       <c r="A107" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B107" s="4">
-        <v>5756</v>
+      <c r="B107" s="6" t="s">
+        <v>1174</v>
       </c>
       <c r="C107" s="3" t="s">
         <v>5</v>
@@ -5461,8 +5911,8 @@
       <c r="A108" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B108" s="4">
-        <v>5761</v>
+      <c r="B108" s="6" t="s">
+        <v>1175</v>
       </c>
       <c r="C108" s="3" t="s">
         <v>5</v>
@@ -5478,8 +5928,8 @@
       <c r="A109" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B109" s="4">
-        <v>5789</v>
+      <c r="B109" s="6" t="s">
+        <v>1176</v>
       </c>
       <c r="C109" s="3" t="s">
         <v>5</v>
@@ -5495,8 +5945,8 @@
       <c r="A110" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B110" s="4">
-        <v>5790</v>
+      <c r="B110" s="6" t="s">
+        <v>1177</v>
       </c>
       <c r="C110" s="3" t="s">
         <v>5</v>
@@ -5512,8 +5962,8 @@
       <c r="A111" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B111" s="4">
-        <v>5792</v>
+      <c r="B111" s="6" t="s">
+        <v>1178</v>
       </c>
       <c r="C111" s="3" t="s">
         <v>5</v>
@@ -5529,8 +5979,8 @@
       <c r="A112" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B112" s="4">
-        <v>5809</v>
+      <c r="B112" s="6" t="s">
+        <v>1179</v>
       </c>
       <c r="C112" s="3" t="s">
         <v>5</v>
@@ -5546,8 +5996,8 @@
       <c r="A113" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B113" s="4">
-        <v>5819</v>
+      <c r="B113" s="6" t="s">
+        <v>1180</v>
       </c>
       <c r="C113" s="3" t="s">
         <v>5</v>
@@ -5563,8 +6013,8 @@
       <c r="A114" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B114" s="4">
-        <v>5837</v>
+      <c r="B114" s="6" t="s">
+        <v>1181</v>
       </c>
       <c r="C114" s="3" t="s">
         <v>5</v>
@@ -5580,8 +6030,8 @@
       <c r="A115" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B115" s="4">
-        <v>5842</v>
+      <c r="B115" s="6" t="s">
+        <v>1182</v>
       </c>
       <c r="C115" s="3" t="s">
         <v>5</v>
@@ -5597,8 +6047,8 @@
       <c r="A116" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B116" s="4">
-        <v>5847</v>
+      <c r="B116" s="6" t="s">
+        <v>1183</v>
       </c>
       <c r="C116" s="3" t="s">
         <v>5</v>
@@ -5614,8 +6064,8 @@
       <c r="A117" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B117" s="4">
-        <v>5854</v>
+      <c r="B117" s="6" t="s">
+        <v>1184</v>
       </c>
       <c r="C117" s="3" t="s">
         <v>5</v>
@@ -5631,8 +6081,8 @@
       <c r="A118" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B118" s="4">
-        <v>5856</v>
+      <c r="B118" s="6" t="s">
+        <v>1185</v>
       </c>
       <c r="C118" s="3" t="s">
         <v>5</v>
@@ -5648,8 +6098,8 @@
       <c r="A119" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B119" s="4">
-        <v>5858</v>
+      <c r="B119" s="6" t="s">
+        <v>1186</v>
       </c>
       <c r="C119" s="3" t="s">
         <v>5</v>
@@ -5665,8 +6115,8 @@
       <c r="A120" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B120" s="4">
-        <v>5861</v>
+      <c r="B120" s="6" t="s">
+        <v>1187</v>
       </c>
       <c r="C120" s="3" t="s">
         <v>5</v>
@@ -5682,8 +6132,8 @@
       <c r="A121" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B121" s="4">
-        <v>5873</v>
+      <c r="B121" s="6" t="s">
+        <v>1188</v>
       </c>
       <c r="C121" s="3" t="s">
         <v>5</v>
@@ -5699,8 +6149,8 @@
       <c r="A122" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B122" s="4">
-        <v>5885</v>
+      <c r="B122" s="6" t="s">
+        <v>1189</v>
       </c>
       <c r="C122" s="3" t="s">
         <v>5</v>
@@ -5716,8 +6166,8 @@
       <c r="A123" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B123" s="4">
-        <v>5887</v>
+      <c r="B123" s="6" t="s">
+        <v>1190</v>
       </c>
       <c r="C123" s="3" t="s">
         <v>5</v>
@@ -5733,8 +6183,8 @@
       <c r="A124" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B124" s="4">
-        <v>5890</v>
+      <c r="B124" s="6" t="s">
+        <v>1191</v>
       </c>
       <c r="C124" s="3" t="s">
         <v>5</v>
@@ -5750,8 +6200,8 @@
       <c r="A125" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B125" s="4">
-        <v>5893</v>
+      <c r="B125" s="6" t="s">
+        <v>1192</v>
       </c>
       <c r="C125" s="3" t="s">
         <v>5</v>
@@ -5767,8 +6217,8 @@
       <c r="A126" s="5" t="s">
         <v>1066</v>
       </c>
-      <c r="B126" s="4">
-        <v>5895</v>
+      <c r="B126" s="6" t="s">
+        <v>1193</v>
       </c>
       <c r="C126" s="3" t="s">
         <v>5</v>
@@ -5784,8 +6234,8 @@
       <c r="A127" s="5" t="s">
         <v>1067</v>
       </c>
-      <c r="B127" s="4">
-        <v>8001</v>
+      <c r="B127" s="6" t="s">
+        <v>1194</v>
       </c>
       <c r="C127" s="3" t="s">
         <v>131</v>
@@ -5801,8 +6251,8 @@
       <c r="A128" s="5" t="s">
         <v>1067</v>
       </c>
-      <c r="B128" s="4">
-        <v>8078</v>
+      <c r="B128" s="6" t="s">
+        <v>1195</v>
       </c>
       <c r="C128" s="3" t="s">
         <v>131</v>
@@ -5818,8 +6268,8 @@
       <c r="A129" s="5" t="s">
         <v>1067</v>
       </c>
-      <c r="B129" s="4">
-        <v>8137</v>
+      <c r="B129" s="6" t="s">
+        <v>1196</v>
       </c>
       <c r="C129" s="3" t="s">
         <v>131</v>
@@ -5835,8 +6285,8 @@
       <c r="A130" s="5" t="s">
         <v>1067</v>
       </c>
-      <c r="B130" s="4">
-        <v>8141</v>
+      <c r="B130" s="6" t="s">
+        <v>1197</v>
       </c>
       <c r="C130" s="3" t="s">
         <v>131</v>
@@ -5852,8 +6302,8 @@
       <c r="A131" s="5" t="s">
         <v>1067</v>
       </c>
-      <c r="B131" s="4">
-        <v>8296</v>
+      <c r="B131" s="6" t="s">
+        <v>1198</v>
       </c>
       <c r="C131" s="3" t="s">
         <v>131</v>
@@ -5869,8 +6319,8 @@
       <c r="A132" s="5" t="s">
         <v>1067</v>
       </c>
-      <c r="B132" s="4">
-        <v>8372</v>
+      <c r="B132" s="6" t="s">
+        <v>1199</v>
       </c>
       <c r="C132" s="3" t="s">
         <v>131</v>
@@ -5886,8 +6336,8 @@
       <c r="A133" s="5" t="s">
         <v>1067</v>
       </c>
-      <c r="B133" s="4">
-        <v>8421</v>
+      <c r="B133" s="6" t="s">
+        <v>1200</v>
       </c>
       <c r="C133" s="3" t="s">
         <v>131</v>
@@ -5903,8 +6353,8 @@
       <c r="A134" s="5" t="s">
         <v>1067</v>
       </c>
-      <c r="B134" s="4">
-        <v>8433</v>
+      <c r="B134" s="6" t="s">
+        <v>1201</v>
       </c>
       <c r="C134" s="3" t="s">
         <v>131</v>
@@ -5920,8 +6370,8 @@
       <c r="A135" s="5" t="s">
         <v>1067</v>
       </c>
-      <c r="B135" s="4">
-        <v>8436</v>
+      <c r="B135" s="6" t="s">
+        <v>1202</v>
       </c>
       <c r="C135" s="3" t="s">
         <v>131</v>
@@ -5937,8 +6387,8 @@
       <c r="A136" s="5" t="s">
         <v>1067</v>
       </c>
-      <c r="B136" s="4">
-        <v>8520</v>
+      <c r="B136" s="6" t="s">
+        <v>1203</v>
       </c>
       <c r="C136" s="3" t="s">
         <v>131</v>
@@ -5954,8 +6404,8 @@
       <c r="A137" s="5" t="s">
         <v>1067</v>
       </c>
-      <c r="B137" s="4">
-        <v>8549</v>
+      <c r="B137" s="6" t="s">
+        <v>1204</v>
       </c>
       <c r="C137" s="3" t="s">
         <v>131</v>
@@ -5971,8 +6421,8 @@
       <c r="A138" s="5" t="s">
         <v>1067</v>
       </c>
-      <c r="B138" s="4">
-        <v>8558</v>
+      <c r="B138" s="6" t="s">
+        <v>1205</v>
       </c>
       <c r="C138" s="3" t="s">
         <v>131</v>
@@ -5988,8 +6438,8 @@
       <c r="A139" s="5" t="s">
         <v>1067</v>
       </c>
-      <c r="B139" s="4">
-        <v>8560</v>
+      <c r="B139" s="6" t="s">
+        <v>1206</v>
       </c>
       <c r="C139" s="3" t="s">
         <v>131</v>
@@ -6005,8 +6455,8 @@
       <c r="A140" s="5" t="s">
         <v>1067</v>
       </c>
-      <c r="B140" s="4">
-        <v>8573</v>
+      <c r="B140" s="6" t="s">
+        <v>1207</v>
       </c>
       <c r="C140" s="3" t="s">
         <v>131</v>
@@ -6022,8 +6472,8 @@
       <c r="A141" s="5" t="s">
         <v>1067</v>
       </c>
-      <c r="B141" s="4">
-        <v>8606</v>
+      <c r="B141" s="6" t="s">
+        <v>1208</v>
       </c>
       <c r="C141" s="3" t="s">
         <v>131</v>
@@ -6039,8 +6489,8 @@
       <c r="A142" s="5" t="s">
         <v>1067</v>
       </c>
-      <c r="B142" s="4">
-        <v>8634</v>
+      <c r="B142" s="6" t="s">
+        <v>1209</v>
       </c>
       <c r="C142" s="3" t="s">
         <v>131</v>
@@ -6056,8 +6506,8 @@
       <c r="A143" s="5" t="s">
         <v>1067</v>
       </c>
-      <c r="B143" s="4">
-        <v>8638</v>
+      <c r="B143" s="6" t="s">
+        <v>1210</v>
       </c>
       <c r="C143" s="3" t="s">
         <v>131</v>
@@ -6073,8 +6523,8 @@
       <c r="A144" s="5" t="s">
         <v>1067</v>
       </c>
-      <c r="B144" s="4">
-        <v>8675</v>
+      <c r="B144" s="6" t="s">
+        <v>1211</v>
       </c>
       <c r="C144" s="3" t="s">
         <v>131</v>
@@ -6090,8 +6540,8 @@
       <c r="A145" s="5" t="s">
         <v>1067</v>
       </c>
-      <c r="B145" s="4">
-        <v>8685</v>
+      <c r="B145" s="6" t="s">
+        <v>1212</v>
       </c>
       <c r="C145" s="3" t="s">
         <v>131</v>
@@ -6107,8 +6557,8 @@
       <c r="A146" s="5" t="s">
         <v>1067</v>
       </c>
-      <c r="B146" s="4">
-        <v>8758</v>
+      <c r="B146" s="6" t="s">
+        <v>1213</v>
       </c>
       <c r="C146" s="3" t="s">
         <v>131</v>
@@ -6124,8 +6574,8 @@
       <c r="A147" s="5" t="s">
         <v>1067</v>
       </c>
-      <c r="B147" s="4">
-        <v>8770</v>
+      <c r="B147" s="6" t="s">
+        <v>1214</v>
       </c>
       <c r="C147" s="3" t="s">
         <v>131</v>
@@ -6141,8 +6591,8 @@
       <c r="A148" s="5" t="s">
         <v>1067</v>
       </c>
-      <c r="B148" s="4">
-        <v>8832</v>
+      <c r="B148" s="6" t="s">
+        <v>1215</v>
       </c>
       <c r="C148" s="3" t="s">
         <v>131</v>
@@ -6158,8 +6608,8 @@
       <c r="A149" s="5" t="s">
         <v>1067</v>
       </c>
-      <c r="B149" s="4">
-        <v>8849</v>
+      <c r="B149" s="6" t="s">
+        <v>1216</v>
       </c>
       <c r="C149" s="3" t="s">
         <v>131</v>

</xml_diff>